<commit_message>
Added Mariam's config and updated Rscript to parse them
</commit_message>
<xml_diff>
--- a/TimeVizConfigdoc.xlsx
+++ b/TimeVizConfigdoc.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">The Output PDF should be the file location/name of the Output PDF. As shown in the example to the right:</t>
   </si>
   <si>
-    <t xml:space="preserve">Users/ashst/OneDrive/Documents/Capstone for Biotechnology/ABCDEFG3.pdf</t>
+    <t xml:space="preserve">/Users/MZ/Downloads/Example.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Output Height</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">The list of tracks also known as the order of the tracks to plot the top to the bottom. The Track Type is often composed of the sheet names from spreadsheet and separated by semicolons. Such as the example on the right: </t>
   </si>
   <si>
-    <t xml:space="preserve">TimeTrack1;DataTrack1;DataTrack2;DataTrack3;DetailsAnnotation;AnnotationTrack1;AnnotationTrack2</t>
+    <t xml:space="preserve">TimeTrack1;DataTrack1;DataTrack2;DataTrack3;AnnotationTrack1;AnnotationTrack2</t>
   </si>
   <si>
     <t xml:space="preserve">Track Type</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">This package is set to come up with acceptable defaults for the axis annotation. This feature can be adjusted through the exponent parameter, which takes an integer value greater then zero. There are different options for Track Types in this package for example data annotations, time, etc. However, all of these values must be separated by a semicolon as seen in the example to the right.</t>
   </si>
   <si>
-    <t xml:space="preserve">time;data;data;data;annotation;annotation;annotation</t>
+    <t xml:space="preserve">time;data;data;data;annotation;annotation</t>
   </si>
   <si>
     <t xml:space="preserve">Track Heights</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">The heights for each track are relative to the sum across tracks for example (ie: 1;3;3 = 1/7th of total height;3/7ths of total height;3/7ths of total height). A semicolon is required to separate the values as shown in the example to the right: </t>
   </si>
   <si>
-    <t xml:space="preserve">2;2;2;2;2;2;2</t>
+    <t xml:space="preserve">2;4;4;4;8;6</t>
   </si>
   <si>
     <t xml:space="preserve">Track Names</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">The Track Names are the names to be printed with each track, and must be separated by a semicolon. The default value for this category is the sheet names from the spreadsheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Seconds;Protein Production\n(kDa/ns);% Protein\nCorrectly Folded;Available Glycosylation\nSites;Protein Production\n Details;Sub-Events;Events</t>
+    <t xml:space="preserve">Seconds;Protein Production\n(kDa/ns);% Protein\nCorrectly Folded;Available Glycosylation\nSites;Sub-Events;Events</t>
   </si>
   <si>
     <t xml:space="preserve">Track Box Color</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">The Track Box Color is the color that will be printed inside of the box, with a default value being set to gray. Other options can be selected, but must be separated by a semi colon. </t>
   </si>
   <si>
-    <t xml:space="preserve">white;orange;orange;orange;orange;forestgreen;forestgreen</t>
+    <t xml:space="preserve">white;orange;orange;orange;forestgreen;forestgreen</t>
   </si>
   <si>
     <t xml:space="preserve">Track Background Color</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">The Track Background Color is the color of the track background.</t>
   </si>
   <si>
-    <t xml:space="preserve">white;white;white;white;white;white;white</t>
+    <t xml:space="preserve">white;white;white;white;white;white</t>
   </si>
   <si>
     <t xml:space="preserve">Track Label Color</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">The Track Label Size is the font size for each title label, and must be separated by a semicolon. </t>
   </si>
   <si>
-    <t xml:space="preserve">0.2;0.6;0.6;0.6;0.6;0.45;0.6</t>
+    <t xml:space="preserve">0.6;0.6;0.6;0.45;0.6;0.6</t>
   </si>
   <si>
     <t xml:space="preserve">Data Type</t>
@@ -488,8 +488,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -609,17 +610,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -631,14 +628,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -765,405 +762,399 @@
   </sheetPr>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="23.93"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="2" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="78" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C21" s="6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C22" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="2" t="n">
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="C24" s="6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C28" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C29" s="6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C35" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1189,49 +1180,49 @@
       <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1749,46 +1740,46 @@
       <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2019,46 +2010,46 @@
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="7" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2289,7 +2280,7 @@
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.9"/>
   </cols>
@@ -2418,199 +2409,199 @@
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="31.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="31.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="19.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="7" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="11" t="n">
+      <c r="E4" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="11" t="n">
+      <c r="E5" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E6" s="11" t="n">
+      <c r="E6" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="11" t="n">
+      <c r="E7" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="11" t="n">
+      <c r="E9" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="11" t="n">
+      <c r="E10" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="11" t="n">
+      <c r="E11" s="10" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -2636,7 +2627,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30"/>
@@ -2645,71 +2636,71 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.3"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="7" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="16" t="n">
+      <c r="E2" s="15" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="16" t="n">
+      <c r="E3" s="15" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="16" t="n">
+      <c r="E4" s="15" t="n">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>